<commit_message>
added df last and looping
</commit_message>
<xml_diff>
--- a/excel_list/englishNameTranslate/dictionary_space.xlsx
+++ b/excel_list/englishNameTranslate/dictionary_space.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adipr\PycharmProjects\englishTranslate\excel_list\englishNameTranslate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0C0D6E-FD47-48F6-96E4-CBDEAD76C6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A570E186-7A50-426F-898B-79DAEE363CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="202">
   <si>
     <t>Japanese</t>
   </si>
@@ -596,18 +596,67 @@
   </si>
   <si>
     <t>Melon Bread</t>
+  </si>
+  <si>
+    <t>ピノ</t>
+  </si>
+  <si>
+    <t>Pino</t>
+  </si>
+  <si>
+    <t>ごつ盛り</t>
+  </si>
+  <si>
+    <t>Gotsumori</t>
+  </si>
+  <si>
+    <t>ハッピーターン</t>
+  </si>
+  <si>
+    <t>Happy Turn</t>
+  </si>
+  <si>
+    <t>カラムーチョ</t>
+  </si>
+  <si>
+    <t>Karamucho</t>
+  </si>
+  <si>
+    <t>ビーノ</t>
+  </si>
+  <si>
+    <t>Beano</t>
+  </si>
+  <si>
+    <t>ラテ</t>
+  </si>
+  <si>
+    <t>Latte</t>
+  </si>
+  <si>
+    <t>リアルゴールド</t>
+  </si>
+  <si>
+    <t>Real Gold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="69">
+  <fonts count="70">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1139,38 +1188,38 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1180,8 +1229,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1190,7 +1242,7 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1211,214 +1263,217 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1428,27 +1483,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1458,18 +1513,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1479,32 +1531,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1834,8 +1886,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H2296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15"/>
@@ -2615,34 +2667,75 @@
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>189</v>
+      </c>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="2:8">
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>191</v>
+      </c>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="2:8">
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>192</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>193</v>
+      </c>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="2:8">
+    <row r="99" spans="1:8">
+      <c r="A99" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" s="120" t="s">
+        <v>195</v>
+      </c>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="2:8">
+    <row r="100" spans="1:8">
+      <c r="A100" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B100" s="120" t="s">
+        <v>197</v>
+      </c>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="2:8">
+    <row r="101" spans="1:8">
+      <c r="A101" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" s="120" t="s">
+        <v>199</v>
+      </c>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="2:8">
-      <c r="B102" s="48"/>
+    <row r="102" spans="1:8">
+      <c r="A102" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="126" t="s">
+        <v>201</v>
+      </c>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="2:8">
+    <row r="103" spans="1:8">
       <c r="H103" s="3"/>
     </row>
-    <row r="108" spans="2:8">
+    <row r="108" spans="1:8">
       <c r="B108" s="50"/>
     </row>
-    <row r="111" spans="2:8">
+    <row r="111" spans="1:8">
       <c r="B111" s="41"/>
     </row>
     <row r="114" spans="1:2">

</xml_diff>